<commit_message>
new DTO extractions added
</commit_message>
<xml_diff>
--- a/data/DTO extractions/Pop_Coords2024_with_GLORYS_info.xlsx
+++ b/data/DTO extractions/Pop_Coords2024_with_GLORYS_info.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stanleyr\Documents\Github\SnowCrabGenomics\data\DTO extractions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEFFERYN\Documents\GitHub\SnowCrabGenomics\data\DTO extractions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6524CA72-1E27-486B-812A-BDAEC468C63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F64690-B1A9-4A4B-9415-93638E1D9C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="15" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>SampleSite</t>
   </si>
@@ -304,6 +304,24 @@
   </si>
   <si>
     <t>Northeast Nova Scotia outer</t>
+  </si>
+  <si>
+    <t>locations_nc_2025_newpointsonly/GLORYS_monthly_Laur_Chn._v2_1993_2024.nc</t>
+  </si>
+  <si>
+    <t>R557</t>
+  </si>
+  <si>
+    <t>Laur Chn.</t>
+  </si>
+  <si>
+    <t>locations_nc_2025_newpointsonly/GLORYS_monthly_CMA_10A_v2_1993_2024.nc</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>CMA 10A</t>
   </si>
 </sst>
 </file>
@@ -659,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +692,7 @@
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1606,6 +1624,70 @@
         <v>91</v>
       </c>
     </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30">
+        <v>46.749833000000002</v>
+      </c>
+      <c r="D30">
+        <v>-54.832166999999998</v>
+      </c>
+      <c r="E30">
+        <v>-54.833300000000001</v>
+      </c>
+      <c r="F30">
+        <v>46.75</v>
+      </c>
+      <c r="G30">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H30">
+        <v>25</v>
+      </c>
+      <c r="I30">
+        <v>155.89999389648438</v>
+      </c>
+      <c r="J30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31">
+        <v>46.333333330000002</v>
+      </c>
+      <c r="D31">
+        <v>-57.251166670000003</v>
+      </c>
+      <c r="E31">
+        <v>-57.25</v>
+      </c>
+      <c r="F31">
+        <v>46.333300000000001</v>
+      </c>
+      <c r="G31">
+        <v>0.09</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+      <c r="I31">
+        <v>380.20001220703125</v>
+      </c>
+      <c r="J31" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>